<commit_message>
updated the XPath Cheat Sheet
</commit_message>
<xml_diff>
--- a/PageObjectFramework/Resources/XPathCheatSheet.xlsx
+++ b/PageObjectFramework/Resources/XPathCheatSheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
   <si>
     <t>//*</t>
   </si>
@@ -101,9 +101,6 @@
     <t>(n)th element (*)</t>
   </si>
   <si>
-    <t>children elements</t>
-  </si>
-  <si>
     <t>parent elements</t>
   </si>
   <si>
@@ -153,6 +150,27 @@
   </si>
   <si>
     <t>(n)th element (more in-depth)</t>
+  </si>
+  <si>
+    <t>//*//*</t>
+  </si>
+  <si>
+    <t>//td//img</t>
+  </si>
+  <si>
+    <t>&lt;tr&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img&gt;&lt;/img&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/tr&gt;</t>
+  </si>
+  <si>
+    <t>direct child</t>
+  </si>
+  <si>
+    <t>child of child</t>
   </si>
 </sst>
 </file>
@@ -176,7 +194,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -186,6 +204,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -202,10 +226,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -489,10 +514,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:I43"/>
+  <dimension ref="B1:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J53" sqref="J53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,24 +527,25 @@
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="37.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.7109375" customWidth="1"/>
-    <col min="9" max="9" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.85546875" customWidth="1"/>
+    <col min="10" max="10" width="32.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -530,7 +556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>2</v>
       </c>
@@ -544,20 +570,21 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>20</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>4</v>
       </c>
@@ -571,20 +598,21 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>23</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>7</v>
       </c>
@@ -598,72 +626,76 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="I17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="I18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="I19" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J19" s="1"/>
+      <c r="K19" s="3"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H20" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>8</v>
       </c>
       <c r="D23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F23" t="s">
+        <v>39</v>
+      </c>
+      <c r="H23" t="s">
         <v>40</v>
       </c>
-      <c r="H23" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="I24" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H26" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I26" s="1"/>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J26" s="1"/>
+      <c r="K26" s="3"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="I27" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H28" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>17</v>
       </c>
       <c r="D31" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="F31" t="s">
         <v>18</v>
@@ -672,70 +704,110 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="I32" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J32" s="1"/>
+      <c r="K32" s="3"/>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H33" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36" t="s">
+        <v>48</v>
+      </c>
+      <c r="F36" t="s">
+        <v>43</v>
+      </c>
+      <c r="H36" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I37" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="J38" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K38" s="3"/>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I39" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H40" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
         <v>19</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D43" t="s">
+        <v>25</v>
+      </c>
+      <c r="F43" t="s">
         <v>26</v>
       </c>
-      <c r="F36" t="s">
+      <c r="H43" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="3"/>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I44" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H45" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
         <v>27</v>
       </c>
-      <c r="H36" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I36" s="1"/>
-    </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="I37" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H38" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
+      <c r="D48" t="s">
         <v>28</v>
       </c>
-      <c r="D41" t="s">
+      <c r="F48" t="s">
         <v>29</v>
       </c>
-      <c r="F41" t="s">
+      <c r="H48" t="s">
         <v>30</v>
       </c>
-      <c r="H41" t="s">
+    </row>
+    <row r="49" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
+        <v>33</v>
+      </c>
+      <c r="H49" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D42" t="s">
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+    </row>
+    <row r="50" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
         <v>34</v>
       </c>
-      <c r="H42" s="1" t="s">
+      <c r="H50" t="s">
         <v>32</v>
-      </c>
-      <c r="I42" s="1"/>
-    </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D43" t="s">
-        <v>35</v>
-      </c>
-      <c r="H43" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>